<commit_message>
EndophilinA1 was missing and added
</commit_message>
<xml_diff>
--- a/SourceData/AH_sequences.xlsx
+++ b/SourceData/AH_sequences.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://yaleedu-my.sharepoint.com/personal/shoken_lee_yale_edu/Documents/DATA/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shokenlee/Desktop/git/AH_AAcomposition/SourceData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="8_{D550ED7C-C400-3D46-93C0-9577CCBDF7FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{046E7CD2-0B01-0349-A471-ADB913616D6B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5952DB5-4BC1-804F-AA39-0E9E93B7027C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{26EB4E71-CE00-5947-979C-1BB92A1067AA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="82">
   <si>
     <t>EHPIQWLYITCRKVCKG</t>
   </si>
@@ -276,6 +276,12 @@
   </si>
   <si>
     <t>VEEQSKEFVQQVEEKSIDLIQKWEEKSREFIGSFLEMFG</t>
+  </si>
+  <si>
+    <t>EndophilinA1</t>
+  </si>
+  <si>
+    <t>SVAGLKKQFHKATQKVSEKV</t>
   </si>
 </sst>
 </file>
@@ -655,10 +661,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71224647-F2A0-9245-87A2-F683F7D78F3E}">
-  <dimension ref="A1:C41"/>
+  <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1118,6 +1124,17 @@
         <v>1</v>
       </c>
     </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>81</v>
+      </c>
+      <c r="B42" t="s">
+        <v>80</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
SpoVM,Magainin2,GMAP210 added to AH list
</commit_message>
<xml_diff>
--- a/SourceData/AH_sequences.xlsx
+++ b/SourceData/AH_sequences.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shokenlee/Desktop/git/AH_AAcomposition/SourceData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5952DB5-4BC1-804F-AA39-0E9E93B7027C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C747A2F-7477-6643-ACA4-E13520161072}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{26EB4E71-CE00-5947-979C-1BB92A1067AA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="88">
   <si>
     <t>EHPIQWLYITCRKVCKG</t>
   </si>
@@ -282,6 +282,24 @@
   </si>
   <si>
     <t>SVAGLKKQFHKATQKVSEKV</t>
+  </si>
+  <si>
+    <t>Magainin2</t>
+  </si>
+  <si>
+    <t>SpoVM</t>
+  </si>
+  <si>
+    <t>GMAP210</t>
+  </si>
+  <si>
+    <t>MKFYTIKLPKFLGGIVRAMLGSFRKD</t>
+  </si>
+  <si>
+    <t>MSSWLGGLGSGLGQSLGQVGGSLASLTGQISNFTKDML</t>
+  </si>
+  <si>
+    <t>GIGKFLHSAKKFGKAFVGEIMNS</t>
   </si>
 </sst>
 </file>
@@ -661,10 +679,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71224647-F2A0-9245-87A2-F683F7D78F3E}">
-  <dimension ref="A1:C42"/>
+  <dimension ref="A1:C45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1135,6 +1153,39 @@
         <v>1</v>
       </c>
     </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>85</v>
+      </c>
+      <c r="B43" t="s">
+        <v>83</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>87</v>
+      </c>
+      <c r="B44" t="s">
+        <v>82</v>
+      </c>
+      <c r="C44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>86</v>
+      </c>
+      <c r="B45" t="s">
+        <v>84</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Sar1 and Arf1 AH NEES data added
</commit_message>
<xml_diff>
--- a/SourceData/AH_sequences.xlsx
+++ b/SourceData/AH_sequences.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shokenlee/Desktop/git/AH_AAcomposition/SourceData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C747A2F-7477-6643-ACA4-E13520161072}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90CF13F9-FB5D-0B4D-9DE8-C3E52196D557}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{26EB4E71-CE00-5947-979C-1BB92A1067AA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="92">
   <si>
     <t>EHPIQWLYITCRKVCKG</t>
   </si>
@@ -300,6 +300,18 @@
   </si>
   <si>
     <t>GIGKFLHSAKKFGKAFVGEIMNS</t>
+  </si>
+  <si>
+    <t>Sar1</t>
+  </si>
+  <si>
+    <t>Arf1</t>
+  </si>
+  <si>
+    <t>MGNIFANLFKGLFGKKE</t>
+  </si>
+  <si>
+    <t>MAGWDIFGWFRDVLASLGLWNKH</t>
   </si>
 </sst>
 </file>
@@ -679,10 +691,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71224647-F2A0-9245-87A2-F683F7D78F3E}">
-  <dimension ref="A1:C45"/>
+  <dimension ref="A1:C47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1186,6 +1198,28 @@
         <v>1</v>
       </c>
     </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>91</v>
+      </c>
+      <c r="B46" t="s">
+        <v>88</v>
+      </c>
+      <c r="C46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>90</v>
+      </c>
+      <c r="B47" t="s">
+        <v>89</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added AH category column in the source data: 1 ER/Golgi, 2 ER+Mito, 3 Mito, 4 Known, 0 Man1 and Mboat7-2
</commit_message>
<xml_diff>
--- a/SourceData/AH_sequences.xlsx
+++ b/SourceData/AH_sequences.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shokenlee/Desktop/git/AH_AAcomposition/SourceData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90CF13F9-FB5D-0B4D-9DE8-C3E52196D557}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77F06823-1C2C-EE42-96B6-5CF3916A2984}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{26EB4E71-CE00-5947-979C-1BB92A1067AA}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="24940" windowHeight="21100" xr2:uid="{26EB4E71-CE00-5947-979C-1BB92A1067AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$47</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="93">
   <si>
     <t>EHPIQWLYITCRKVCKG</t>
   </si>
@@ -312,6 +315,9 @@
   </si>
   <si>
     <t>MAGWDIFGWFRDVLASLGLWNKH</t>
+  </si>
+  <si>
+    <t>Category</t>
   </si>
 </sst>
 </file>
@@ -691,10 +697,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71224647-F2A0-9245-87A2-F683F7D78F3E}">
-  <dimension ref="A1:C47"/>
+  <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -703,7 +709,7 @@
     <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>65</v>
       </c>
@@ -713,382 +719,487 @@
       <c r="C1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B12" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="1" t="s">
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="C15">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B25" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>29</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B26" t="s">
         <v>30</v>
       </c>
-      <c r="C17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>31</v>
-      </c>
-      <c r="B18" t="s">
-        <v>32</v>
-      </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19" t="s">
-        <v>34</v>
-      </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>35</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B27" t="s">
         <v>36</v>
       </c>
-      <c r="C20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>37</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B28" t="s">
         <v>38</v>
       </c>
-      <c r="C21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>43</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B29" t="s">
         <v>44</v>
       </c>
-      <c r="C24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C25">
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C32">
         <v>2</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>46</v>
-      </c>
-      <c r="B26" t="s">
-        <v>47</v>
-      </c>
-      <c r="C26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>48</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C30">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+      <c r="D32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
         <v>55</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B33" t="s">
         <v>56</v>
       </c>
-      <c r="C31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B34" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
         <v>61</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B35" t="s">
         <v>62</v>
       </c>
-      <c r="C34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>63</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>64</v>
-      </c>
       <c r="C35">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>74</v>
       </c>
@@ -1098,8 +1209,11 @@
       <c r="C36">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D36">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>75</v>
       </c>
@@ -1109,8 +1223,11 @@
       <c r="C37">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D37">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>76</v>
       </c>
@@ -1120,8 +1237,11 @@
       <c r="C38">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D38">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>77</v>
       </c>
@@ -1131,8 +1251,11 @@
       <c r="C39">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D39">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>78</v>
       </c>
@@ -1142,8 +1265,11 @@
       <c r="C40">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D40">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>79</v>
       </c>
@@ -1153,8 +1279,11 @@
       <c r="C41">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D41">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>81</v>
       </c>
@@ -1164,8 +1293,11 @@
       <c r="C42">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D42">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>85</v>
       </c>
@@ -1175,8 +1307,11 @@
       <c r="C43">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D43">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>87</v>
       </c>
@@ -1186,8 +1321,11 @@
       <c r="C44">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D44">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>86</v>
       </c>
@@ -1197,8 +1335,11 @@
       <c r="C45">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D45">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>91</v>
       </c>
@@ -1208,8 +1349,11 @@
       <c r="C46">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D46">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>90</v>
       </c>
@@ -1219,8 +1363,16 @@
       <c r="C47">
         <v>1</v>
       </c>
+      <c r="D47">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D47" xr:uid="{71224647-F2A0-9245-87A2-F683F7D78F3E}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D47">
+      <sortCondition ref="D1:D47"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
KDSR was retained in the output with NEES raw and transformed values left NaN
</commit_message>
<xml_diff>
--- a/SourceData/AH_sequences.xlsx
+++ b/SourceData/AH_sequences.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shokenlee/Desktop/git/AH_AAcomposition/SourceData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77F06823-1C2C-EE42-96B6-5CF3916A2984}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91D403A6-A422-B742-A507-087C5D4F3104}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="24940" windowHeight="21100" xr2:uid="{26EB4E71-CE00-5947-979C-1BB92A1067AA}"/>
   </bookViews>
@@ -700,7 +700,7 @@
   <dimension ref="A1:D47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -734,7 +734,7 @@
         <v>2</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
SGPP1 and EMC1 now in category 2
</commit_message>
<xml_diff>
--- a/SourceData/AH_sequences.xlsx
+++ b/SourceData/AH_sequences.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shokenlee/Desktop/git/AH_AAcomposition/SourceData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91D403A6-A422-B742-A507-087C5D4F3104}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73C48C43-5B9E-B147-AD09-637AD7CD768D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="24940" windowHeight="21100" xr2:uid="{26EB4E71-CE00-5947-979C-1BB92A1067AA}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="24940" windowHeight="18360" xr2:uid="{26EB4E71-CE00-5947-979C-1BB92A1067AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -699,8 +699,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71224647-F2A0-9245-87A2-F683F7D78F3E}">
   <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17:D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -724,31 +724,31 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C2">
+      <c r="C3">
         <v>2</v>
       </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
       <c r="D3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -822,11 +822,11 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>48</v>
+      <c r="A9" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -836,11 +836,11 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>57</v>
+      <c r="A10" t="s">
+        <v>63</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -851,16 +851,16 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -921,38 +921,38 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
       <c r="D16">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B18" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="C17">
-        <v>1</v>
-      </c>
-      <c r="D17">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>10</v>
-      </c>
-      <c r="B18" t="s">
-        <v>11</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -963,24 +963,24 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B20" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
-      <c r="D19">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -991,10 +991,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -1005,10 +1005,10 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -1019,10 +1019,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C23">
         <v>1</v>

</xml_diff>

<commit_message>
Nup133(S17R) and TMEM126A(Mut) added; SpoVM and Epsin1 moved to category 0
</commit_message>
<xml_diff>
--- a/SourceData/AH_sequences.xlsx
+++ b/SourceData/AH_sequences.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10921"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shokenlee/Desktop/git/AH_AAcomposition/SourceData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73C48C43-5B9E-B147-AD09-637AD7CD768D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D98F8FE3-AE1E-4147-81B9-9DA402CFF89E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="24940" windowHeight="18360" xr2:uid="{26EB4E71-CE00-5947-979C-1BB92A1067AA}"/>
+    <workbookView xWindow="3960" yWindow="740" windowWidth="24940" windowHeight="18360" xr2:uid="{26EB4E71-CE00-5947-979C-1BB92A1067AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$47</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$50</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="99">
   <si>
     <t>EHPIQWLYITCRKVCKG</t>
   </si>
@@ -318,6 +318,24 @@
   </si>
   <si>
     <t>Category</t>
+  </si>
+  <si>
+    <t>Nup133(S17R)</t>
+  </si>
+  <si>
+    <t>TMEM126A(R15S)</t>
+  </si>
+  <si>
+    <t>TMEM126A(K11S/R15S)</t>
+  </si>
+  <si>
+    <t>NILSYWIRTSKPVFSKMLFPILL</t>
+  </si>
+  <si>
+    <t>NILSYWIRTSSPVFSKMLFPILL</t>
+  </si>
+  <si>
+    <t>LPQGQGMLSGIGRKVSRLFGILS</t>
   </si>
 </sst>
 </file>
@@ -697,16 +715,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71224647-F2A0-9245-87A2-F683F7D78F3E}">
-  <dimension ref="A1:D47"/>
+  <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17:D35"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -1131,10 +1149,10 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>52</v>
+        <v>96</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>53</v>
+        <v>94</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -1145,24 +1163,24 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>54</v>
+        <v>97</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>1</v>
+        <v>95</v>
       </c>
       <c r="C32">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D32">
         <v>3</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>55</v>
-      </c>
-      <c r="B33" t="s">
-        <v>56</v>
+      <c r="A33" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>53</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -1173,13 +1191,13 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>60</v>
+        <v>1</v>
       </c>
       <c r="C34">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D34">
         <v>3</v>
@@ -1187,10 +1205,10 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B35" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C35">
         <v>1</v>
@@ -1200,39 +1218,39 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>74</v>
-      </c>
-      <c r="B36" t="s">
-        <v>68</v>
+      <c r="A36" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="C36">
         <v>1</v>
       </c>
       <c r="D36">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>75</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>69</v>
+        <v>61</v>
+      </c>
+      <c r="B37" t="s">
+        <v>62</v>
       </c>
       <c r="C37">
         <v>1</v>
       </c>
       <c r="D37">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B38" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C38">
         <v>1</v>
@@ -1243,10 +1261,10 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C39">
         <v>1</v>
@@ -1257,10 +1275,10 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>78</v>
-      </c>
-      <c r="B40" t="s">
-        <v>72</v>
+        <v>98</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>93</v>
       </c>
       <c r="C40">
         <v>1</v>
@@ -1271,10 +1289,10 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>79</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>73</v>
+        <v>76</v>
+      </c>
+      <c r="B41" t="s">
+        <v>70</v>
       </c>
       <c r="C41">
         <v>1</v>
@@ -1285,24 +1303,24 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>81</v>
-      </c>
-      <c r="B42" t="s">
-        <v>80</v>
+        <v>77</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>71</v>
       </c>
       <c r="C42">
         <v>1</v>
       </c>
       <c r="D42">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="B43" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="C43">
         <v>1</v>
@@ -1313,10 +1331,10 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>87</v>
-      </c>
-      <c r="B44" t="s">
-        <v>82</v>
+        <v>79</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>73</v>
       </c>
       <c r="C44">
         <v>1</v>
@@ -1327,10 +1345,10 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B45" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C45">
         <v>1</v>
@@ -1341,24 +1359,24 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B46" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C46">
         <v>1</v>
       </c>
       <c r="D46">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B47" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="C47">
         <v>1</v>
@@ -1367,10 +1385,52 @@
         <v>4</v>
       </c>
     </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>86</v>
+      </c>
+      <c r="B48" t="s">
+        <v>84</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="D48">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>91</v>
+      </c>
+      <c r="B49" t="s">
+        <v>88</v>
+      </c>
+      <c r="C49">
+        <v>1</v>
+      </c>
+      <c r="D49">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>90</v>
+      </c>
+      <c r="B50" t="s">
+        <v>89</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+      <c r="D50">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:D47" xr:uid="{71224647-F2A0-9245-87A2-F683F7D78F3E}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D47">
-      <sortCondition ref="D1:D47"/>
+  <autoFilter ref="A1:D50" xr:uid="{71224647-F2A0-9245-87A2-F683F7D78F3E}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D50">
+      <sortCondition ref="D1:D50"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
ArfGAP1 each ALPS1 and ALPS2 added but the resulting _with heliquest csv is still messy
</commit_message>
<xml_diff>
--- a/SourceData/AH_sequences.xlsx
+++ b/SourceData/AH_sequences.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shokenlee/Desktop/git/AH_AAcomposition/SourceData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D98F8FE3-AE1E-4147-81B9-9DA402CFF89E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8E53BAA-A761-4C49-B32D-EA6460E07536}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3960" yWindow="740" windowWidth="24940" windowHeight="18360" xr2:uid="{26EB4E71-CE00-5947-979C-1BB92A1067AA}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="103">
   <si>
     <t>EHPIQWLYITCRKVCKG</t>
   </si>
@@ -336,6 +336,18 @@
   </si>
   <si>
     <t>LPQGQGMLSGIGRKVSRLFGILS</t>
+  </si>
+  <si>
+    <t>ArfGAP1-AH2</t>
+  </si>
+  <si>
+    <t>ArfGAP1-AH1</t>
+  </si>
+  <si>
+    <t>FLNNAMSSLYSGWSSFTTGASRFASAAKEGATKFGS</t>
+  </si>
+  <si>
+    <t>IFDDVSSGVSQLASKVQGVGSKGWRDVTTFFS</t>
   </si>
 </sst>
 </file>
@@ -715,15 +727,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71224647-F2A0-9245-87A2-F683F7D78F3E}">
-  <dimension ref="A1:D50"/>
+  <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="127.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1424,6 +1436,34 @@
         <v>1</v>
       </c>
       <c r="D50">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>101</v>
+      </c>
+      <c r="B51" t="s">
+        <v>100</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+      <c r="D51">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>102</v>
+      </c>
+      <c r="B52" t="s">
+        <v>99</v>
+      </c>
+      <c r="C52">
+        <v>1</v>
+      </c>
+      <c r="D52">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Sun2 sequence but not NEES yet; fixed AH name disapprear problem
</commit_message>
<xml_diff>
--- a/SourceData/AH_sequences.xlsx
+++ b/SourceData/AH_sequences.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10921"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11026"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shokenlee/Desktop/git/AH_AAcomposition/SourceData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8E53BAA-A761-4C49-B32D-EA6460E07536}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D930077-4075-8643-99AF-4FE7808B6154}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3960" yWindow="740" windowWidth="24940" windowHeight="18360" xr2:uid="{26EB4E71-CE00-5947-979C-1BB92A1067AA}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="105">
   <si>
     <t>EHPIQWLYITCRKVCKG</t>
   </si>
@@ -348,13 +348,19 @@
   </si>
   <si>
     <t>IFDDVSSGVSQLASKVQGVGSKGWRDVTTFFS</t>
+  </si>
+  <si>
+    <t>LRSAVSRAGSLLWMVATSPGRLFRLL</t>
+  </si>
+  <si>
+    <t>Sun2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -368,6 +374,12 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -390,9 +402,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -727,10 +740,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71224647-F2A0-9245-87A2-F683F7D78F3E}">
-  <dimension ref="A1:D52"/>
+  <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1467,6 +1480,20 @@
         <v>4</v>
       </c>
     </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B53" t="s">
+        <v>104</v>
+      </c>
+      <c r="C53">
+        <v>1</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:D50" xr:uid="{71224647-F2A0-9245-87A2-F683F7D78F3E}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D50">

</xml_diff>